<commit_message>
Updated tables, figures and fixed some parts
</commit_message>
<xml_diff>
--- a/inputs/SNP_info.xlsx
+++ b/inputs/SNP_info.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1180" windowWidth="28160" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="1180" windowWidth="28160" windowHeight="15320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="126">
   <si>
     <t>Locus</t>
   </si>
@@ -189,12 +189,6 @@
   </si>
   <si>
     <t>rs273909</t>
-  </si>
-  <si>
-    <t>ADTRP-C6orf105</t>
-  </si>
-  <si>
-    <t>rs6903956</t>
   </si>
   <si>
     <t>PHACTR1</t>
@@ -416,11 +410,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -568,6 +562,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -835,14 +832,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:Q60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" bestFit="1" customWidth="1"/>
@@ -854,7 +851,7 @@
     <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:17">
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
@@ -864,7 +861,7 @@
       <c r="P1" s="9"/>
       <c r="Q1" s="9"/>
     </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:17">
       <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
@@ -872,7 +869,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E2" s="24" t="s">
         <v>2</v>
@@ -895,7 +892,7 @@
       <c r="P2" s="10"/>
       <c r="Q2" s="10"/>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:17">
       <c r="B3" s="15" t="s">
         <v>6</v>
       </c>
@@ -927,7 +924,7 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:17">
       <c r="B4" s="15" t="s">
         <v>10</v>
       </c>
@@ -959,7 +956,7 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17">
       <c r="B5" s="15" t="s">
         <v>13</v>
       </c>
@@ -991,7 +988,7 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17">
       <c r="B6" s="15" t="s">
         <v>16</v>
       </c>
@@ -1023,7 +1020,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17">
       <c r="B7" s="15" t="s">
         <v>18</v>
       </c>
@@ -1055,7 +1052,7 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:17">
       <c r="B8" s="15" t="s">
         <v>20</v>
       </c>
@@ -1087,7 +1084,7 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:17">
       <c r="B9" s="15" t="s">
         <v>22</v>
       </c>
@@ -1119,7 +1116,7 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:17">
       <c r="B10" s="20" t="s">
         <v>24</v>
       </c>
@@ -1151,7 +1148,7 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:17">
       <c r="B11" s="15" t="s">
         <v>26</v>
       </c>
@@ -1183,7 +1180,7 @@
       <c r="P11" s="10"/>
       <c r="Q11" s="13"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17">
       <c r="B12" s="15" t="s">
         <v>28</v>
       </c>
@@ -1203,7 +1200,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="H12" s="25">
-        <f t="shared" ref="H12:H58" si="1">LOG(G12)</f>
+        <f t="shared" ref="H12:H57" si="1">LOG(G12)</f>
         <v>5.3078443483419682E-2</v>
       </c>
       <c r="J12" s="9"/>
@@ -1215,7 +1212,7 @@
       <c r="P12" s="10"/>
       <c r="Q12" s="13"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:17">
       <c r="B13" s="15" t="s">
         <v>30</v>
       </c>
@@ -1247,7 +1244,7 @@
       <c r="P13" s="10"/>
       <c r="Q13" s="13"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17">
       <c r="B14" s="15" t="s">
         <v>32</v>
       </c>
@@ -1279,7 +1276,7 @@
       <c r="P14" s="10"/>
       <c r="Q14" s="13"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:17">
       <c r="B15" s="15" t="s">
         <v>34</v>
       </c>
@@ -1311,7 +1308,7 @@
       <c r="P15" s="10"/>
       <c r="Q15" s="13"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17">
       <c r="B16" s="22" t="s">
         <v>36</v>
       </c>
@@ -1343,12 +1340,12 @@
       <c r="P16" s="10"/>
       <c r="Q16" s="13"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:17">
       <c r="B17" s="15" t="s">
         <v>38</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>39</v>
@@ -1375,12 +1372,12 @@
       <c r="P17" s="10"/>
       <c r="Q17" s="13"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:17">
       <c r="B18" s="15" t="s">
         <v>41</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>40</v>
@@ -1407,7 +1404,7 @@
       <c r="P18" s="10"/>
       <c r="Q18" s="13"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:17">
       <c r="B19" s="15" t="s">
         <v>42</v>
       </c>
@@ -1439,7 +1436,7 @@
       <c r="P19" s="10"/>
       <c r="Q19" s="13"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:17">
       <c r="B20" s="15" t="s">
         <v>44</v>
       </c>
@@ -1471,12 +1468,12 @@
       <c r="P20" s="10"/>
       <c r="Q20" s="13"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:17">
       <c r="B21" s="15" t="s">
         <v>46</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D21" s="24" t="s">
         <v>40</v>
@@ -1503,12 +1500,12 @@
       <c r="P21" s="10"/>
       <c r="Q21" s="13"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:17">
       <c r="B22" s="15" t="s">
         <v>47</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D22" s="24" t="s">
         <v>40</v>
@@ -1535,7 +1532,7 @@
       <c r="P22" s="10"/>
       <c r="Q22" s="13"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:17">
       <c r="B23" s="15" t="s">
         <v>48</v>
       </c>
@@ -1567,7 +1564,7 @@
       <c r="P23" s="10"/>
       <c r="Q23" s="13"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:17">
       <c r="B24" s="23" t="s">
         <v>50</v>
       </c>
@@ -1599,7 +1596,7 @@
       <c r="P24" s="10"/>
       <c r="Q24" s="13"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:17">
       <c r="B25" s="15" t="s">
         <v>52</v>
       </c>
@@ -1631,7 +1628,7 @@
       <c r="P25" s="10"/>
       <c r="Q25" s="13"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:17">
       <c r="B26" s="15" t="s">
         <v>54</v>
       </c>
@@ -1639,20 +1636,20 @@
         <v>55</v>
       </c>
       <c r="D26" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="24" t="s">
-        <v>9</v>
-      </c>
       <c r="F26" s="21">
-        <v>0.35405500000000001</v>
+        <v>0.43160599999999999</v>
       </c>
       <c r="G26" s="24">
-        <v>1</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="H26" s="25">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.6904851336472557E-2</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="1"/>
@@ -1663,7 +1660,7 @@
       <c r="P26" s="10"/>
       <c r="Q26" s="13"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:17">
       <c r="B27" s="15" t="s">
         <v>56</v>
       </c>
@@ -1674,17 +1671,17 @@
         <v>9</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F27" s="21">
-        <v>0.43160599999999999</v>
+        <v>0.82367199999999996</v>
       </c>
       <c r="G27" s="24">
-        <v>1.1399999999999999</v>
+        <v>1.03</v>
       </c>
       <c r="H27" s="25">
         <f t="shared" si="1"/>
-        <v>5.6904851336472557E-2</v>
+        <v>1.2837224705172217E-2</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="1"/>
@@ -1695,7 +1692,7 @@
       <c r="P27" s="10"/>
       <c r="Q27" s="13"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:17">
       <c r="B28" s="15" t="s">
         <v>58</v>
       </c>
@@ -1703,20 +1700,20 @@
         <v>59</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E28" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F28" s="21">
-        <v>0.82367199999999996</v>
+        <v>0.80726200000000004</v>
       </c>
       <c r="G28" s="24">
-        <v>1.03</v>
+        <v>1.07</v>
       </c>
       <c r="H28" s="25">
         <f t="shared" si="1"/>
-        <v>1.2837224705172217E-2</v>
+        <v>2.9383777685209667E-2</v>
       </c>
       <c r="J28" s="9"/>
       <c r="K28" s="1"/>
@@ -1727,7 +1724,7 @@
       <c r="P28" s="10"/>
       <c r="Q28" s="13"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:17">
       <c r="B29" s="15" t="s">
         <v>60</v>
       </c>
@@ -1735,19 +1732,19 @@
         <v>61</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F29" s="21">
-        <v>0.80726200000000004</v>
+        <v>0.69995300000000005</v>
       </c>
       <c r="G29" s="24">
         <v>1.07</v>
       </c>
       <c r="H29" s="25">
-        <f t="shared" si="1"/>
+        <f>LOG(G29)</f>
         <v>2.9383777685209667E-2</v>
       </c>
       <c r="J29" s="9"/>
@@ -1759,7 +1756,7 @@
       <c r="P29" s="10"/>
       <c r="Q29" s="13"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:17">
       <c r="B30" s="15" t="s">
         <v>62</v>
       </c>
@@ -1767,20 +1764,20 @@
         <v>63</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F30" s="21">
-        <v>0.69995300000000005</v>
+        <v>5.6243000000000001E-2</v>
       </c>
       <c r="G30" s="24">
-        <v>1.07</v>
+        <v>1.37</v>
       </c>
       <c r="H30" s="25">
-        <f>LOG(G30)</f>
-        <v>2.9383777685209667E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.13672056715640679</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="1"/>
@@ -1791,7 +1788,7 @@
       <c r="P30" s="10"/>
       <c r="Q30" s="13"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:17">
       <c r="B31" s="15" t="s">
         <v>64</v>
       </c>
@@ -1799,20 +1796,20 @@
         <v>65</v>
       </c>
       <c r="D31" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="24" t="s">
-        <v>12</v>
-      </c>
       <c r="F31" s="21">
-        <v>5.6243000000000001E-2</v>
+        <v>5.9660999999999999E-2</v>
       </c>
       <c r="G31" s="24">
-        <v>1.37</v>
+        <v>1.34</v>
       </c>
       <c r="H31" s="25">
         <f t="shared" si="1"/>
-        <v>0.13672056715640679</v>
+        <v>0.12710479836480765</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="1"/>
@@ -1823,7 +1820,7 @@
       <c r="P31" s="10"/>
       <c r="Q31" s="13"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:17">
       <c r="B32" s="15" t="s">
         <v>66</v>
       </c>
@@ -1831,20 +1828,20 @@
         <v>67</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F32" s="21">
-        <v>5.9660999999999999E-2</v>
+        <v>0.20047000000000001</v>
       </c>
       <c r="G32" s="24">
-        <v>1.34</v>
+        <v>1.08</v>
       </c>
       <c r="H32" s="25">
         <f t="shared" si="1"/>
-        <v>0.12710479836480765</v>
+        <v>3.342375548694973E-2</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="1"/>
@@ -1855,7 +1852,7 @@
       <c r="P32" s="10"/>
       <c r="Q32" s="13"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:17">
       <c r="B33" s="15" t="s">
         <v>68</v>
       </c>
@@ -1863,20 +1860,20 @@
         <v>69</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" s="21">
-        <v>0.20047000000000001</v>
+        <v>0.78272699999999995</v>
       </c>
       <c r="G33" s="24">
-        <v>1.08</v>
+        <v>1.05</v>
       </c>
       <c r="H33" s="25">
         <f t="shared" si="1"/>
-        <v>3.342375548694973E-2</v>
+        <v>2.1189299069938092E-2</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="1"/>
@@ -1887,7 +1884,7 @@
       <c r="P33" s="10"/>
       <c r="Q33" s="13"/>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:17">
       <c r="B34" s="15" t="s">
         <v>70</v>
       </c>
@@ -1901,14 +1898,14 @@
         <v>8</v>
       </c>
       <c r="F34" s="21">
-        <v>0.78272699999999995</v>
+        <v>0.68667500000000004</v>
       </c>
       <c r="G34" s="24">
-        <v>1.05</v>
+        <v>1.08</v>
       </c>
       <c r="H34" s="25">
         <f t="shared" si="1"/>
-        <v>2.1189299069938092E-2</v>
+        <v>3.342375548694973E-2</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="1"/>
@@ -1919,7 +1916,7 @@
       <c r="P34" s="10"/>
       <c r="Q34" s="13"/>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:17">
       <c r="B35" s="15" t="s">
         <v>72</v>
       </c>
@@ -1927,20 +1924,20 @@
         <v>73</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F35" s="21">
-        <v>0.68667500000000004</v>
+        <v>0.85259399999999996</v>
       </c>
       <c r="G35" s="24">
-        <v>1.08</v>
+        <v>1.06</v>
       </c>
       <c r="H35" s="25">
         <f t="shared" si="1"/>
-        <v>3.342375548694973E-2</v>
+        <v>2.5305865264770262E-2</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="1"/>
@@ -1951,7 +1948,7 @@
       <c r="P35" s="10"/>
       <c r="Q35" s="13"/>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:17">
       <c r="B36" s="15" t="s">
         <v>74</v>
       </c>
@@ -1959,20 +1956,20 @@
         <v>75</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F36" s="21">
-        <v>0.85259399999999996</v>
+        <v>0.55139499999999997</v>
       </c>
       <c r="G36" s="24">
-        <v>1.06</v>
+        <v>1.04</v>
       </c>
       <c r="H36" s="25">
         <f t="shared" si="1"/>
-        <v>2.5305865264770262E-2</v>
+        <v>1.703333929878037E-2</v>
       </c>
       <c r="J36" s="9"/>
       <c r="K36" s="1"/>
@@ -1983,7 +1980,7 @@
       <c r="P36" s="10"/>
       <c r="Q36" s="13"/>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:17">
       <c r="B37" s="15" t="s">
         <v>76</v>
       </c>
@@ -1991,20 +1988,20 @@
         <v>77</v>
       </c>
       <c r="D37" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="24" t="s">
-        <v>8</v>
-      </c>
       <c r="F37" s="21">
-        <v>0.55139499999999997</v>
+        <v>0.48866799999999999</v>
       </c>
       <c r="G37" s="24">
-        <v>1.04</v>
+        <v>1.21</v>
       </c>
       <c r="H37" s="25">
         <f t="shared" si="1"/>
-        <v>1.703333929878037E-2</v>
+        <v>8.2785370316450071E-2</v>
       </c>
       <c r="J37" s="9"/>
       <c r="K37" s="1"/>
@@ -2015,7 +2012,7 @@
       <c r="P37" s="10"/>
       <c r="Q37" s="13"/>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:17">
       <c r="B38" s="15" t="s">
         <v>78</v>
       </c>
@@ -2023,20 +2020,20 @@
         <v>79</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F38" s="21">
-        <v>0.48866799999999999</v>
+        <v>0.19087200000000001</v>
       </c>
       <c r="G38" s="24">
-        <v>1.21</v>
+        <v>1.08</v>
       </c>
       <c r="H38" s="25">
         <f t="shared" si="1"/>
-        <v>8.2785370316450071E-2</v>
+        <v>3.342375548694973E-2</v>
       </c>
       <c r="J38" s="9"/>
       <c r="K38" s="1"/>
@@ -2047,7 +2044,7 @@
       <c r="P38" s="10"/>
       <c r="Q38" s="13"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:17">
       <c r="B39" s="15" t="s">
         <v>80</v>
       </c>
@@ -2055,20 +2052,20 @@
         <v>81</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F39" s="21">
-        <v>0.19087200000000001</v>
+        <v>0.41822100000000001</v>
       </c>
       <c r="G39" s="24">
-        <v>1.08</v>
+        <v>1.06</v>
       </c>
       <c r="H39" s="25">
         <f t="shared" si="1"/>
-        <v>3.342375548694973E-2</v>
+        <v>2.5305865264770262E-2</v>
       </c>
       <c r="J39" s="9"/>
       <c r="K39" s="1"/>
@@ -2079,7 +2076,7 @@
       <c r="P39" s="10"/>
       <c r="Q39" s="13"/>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:17">
       <c r="B40" s="15" t="s">
         <v>82</v>
       </c>
@@ -2087,20 +2084,20 @@
         <v>83</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E40" s="24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F40" s="21">
-        <v>0.41822100000000001</v>
+        <v>0.63748499999999997</v>
       </c>
       <c r="G40" s="24">
-        <v>1.06</v>
+        <v>1.08</v>
       </c>
       <c r="H40" s="25">
         <f t="shared" si="1"/>
-        <v>2.5305865264770262E-2</v>
+        <v>3.342375548694973E-2</v>
       </c>
       <c r="J40" s="9"/>
       <c r="K40" s="1"/>
@@ -2111,7 +2108,7 @@
       <c r="P40" s="10"/>
       <c r="Q40" s="13"/>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:17">
       <c r="B41" s="15" t="s">
         <v>84</v>
       </c>
@@ -2119,20 +2116,20 @@
         <v>85</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E41" s="24" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F41" s="21">
-        <v>0.63748499999999997</v>
+        <v>0.36913099999999999</v>
       </c>
       <c r="G41" s="24">
-        <v>1.08</v>
+        <v>1.07</v>
       </c>
       <c r="H41" s="25">
         <f t="shared" si="1"/>
-        <v>3.342375548694973E-2</v>
+        <v>2.9383777685209667E-2</v>
       </c>
       <c r="J41" s="9"/>
       <c r="K41" s="1"/>
@@ -2143,8 +2140,8 @@
       <c r="P41" s="10"/>
       <c r="Q41" s="13"/>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B42" s="15" t="s">
+    <row r="42" spans="2:17">
+      <c r="B42" s="23" t="s">
         <v>86</v>
       </c>
       <c r="C42" s="15" t="s">
@@ -2154,20 +2151,20 @@
         <v>8</v>
       </c>
       <c r="E42" s="24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F42" s="21">
-        <v>0.36913099999999999</v>
+        <v>0.87253000000000003</v>
       </c>
       <c r="G42" s="24">
-        <v>1.07</v>
+        <v>1.08</v>
       </c>
       <c r="H42" s="25">
         <f t="shared" si="1"/>
-        <v>2.9383777685209667E-2</v>
+        <v>3.342375548694973E-2</v>
       </c>
       <c r="J42" s="9"/>
-      <c r="K42" s="1"/>
+      <c r="K42" s="7"/>
       <c r="L42" s="9"/>
       <c r="M42" s="10"/>
       <c r="N42" s="10"/>
@@ -2175,31 +2172,31 @@
       <c r="P42" s="10"/>
       <c r="Q42" s="13"/>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B43" s="23" t="s">
+    <row r="43" spans="2:17">
+      <c r="B43" s="15" t="s">
         <v>88</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>89</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F43" s="21">
-        <v>0.87253000000000003</v>
+        <v>0.32353599999999999</v>
       </c>
       <c r="G43" s="24">
-        <v>1.08</v>
+        <v>1.07</v>
       </c>
       <c r="H43" s="25">
         <f t="shared" si="1"/>
-        <v>3.342375548694973E-2</v>
+        <v>2.9383777685209667E-2</v>
       </c>
       <c r="J43" s="9"/>
-      <c r="K43" s="7"/>
+      <c r="K43" s="1"/>
       <c r="L43" s="9"/>
       <c r="M43" s="10"/>
       <c r="N43" s="10"/>
@@ -2207,7 +2204,7 @@
       <c r="P43" s="10"/>
       <c r="Q43" s="13"/>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:17">
       <c r="B44" s="15" t="s">
         <v>90</v>
       </c>
@@ -2215,20 +2212,20 @@
         <v>91</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E44" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F44" s="21">
-        <v>0.32353599999999999</v>
+        <v>0.18470600000000001</v>
       </c>
       <c r="G44" s="24">
-        <v>1.07</v>
+        <v>1.05</v>
       </c>
       <c r="H44" s="25">
         <f t="shared" si="1"/>
-        <v>2.9383777685209667E-2</v>
+        <v>2.1189299069938092E-2</v>
       </c>
       <c r="J44" s="9"/>
       <c r="K44" s="1"/>
@@ -2239,8 +2236,8 @@
       <c r="P44" s="10"/>
       <c r="Q44" s="13"/>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B45" s="15" t="s">
+    <row r="45" spans="2:17">
+      <c r="B45" s="23" t="s">
         <v>92</v>
       </c>
       <c r="C45" s="15" t="s">
@@ -2250,20 +2247,20 @@
         <v>9</v>
       </c>
       <c r="E45" s="24" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F45" s="21">
-        <v>0.18470600000000001</v>
+        <v>0.20130600000000001</v>
       </c>
       <c r="G45" s="24">
-        <v>1.05</v>
+        <v>1.08</v>
       </c>
       <c r="H45" s="25">
         <f t="shared" si="1"/>
-        <v>2.1189299069938092E-2</v>
+        <v>3.342375548694973E-2</v>
       </c>
       <c r="J45" s="9"/>
-      <c r="K45" s="1"/>
+      <c r="K45" s="7"/>
       <c r="L45" s="9"/>
       <c r="M45" s="10"/>
       <c r="N45" s="10"/>
@@ -2271,7 +2268,7 @@
       <c r="P45" s="10"/>
       <c r="Q45" s="13"/>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:17">
       <c r="B46" s="23" t="s">
         <v>94</v>
       </c>
@@ -2279,20 +2276,20 @@
         <v>95</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E46" s="24" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F46" s="21">
-        <v>0.20130600000000001</v>
+        <v>0.42180800000000002</v>
       </c>
       <c r="G46" s="24">
-        <v>1.08</v>
+        <v>1.07</v>
       </c>
       <c r="H46" s="25">
         <f t="shared" si="1"/>
-        <v>3.342375548694973E-2</v>
+        <v>2.9383777685209667E-2</v>
       </c>
       <c r="J46" s="9"/>
       <c r="K46" s="7"/>
@@ -2303,31 +2300,31 @@
       <c r="P46" s="10"/>
       <c r="Q46" s="13"/>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B47" s="23" t="s">
+    <row r="47" spans="2:17">
+      <c r="B47" s="15" t="s">
         <v>96</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>97</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E47" s="24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F47" s="21">
-        <v>0.42180800000000002</v>
+        <v>0.314419</v>
       </c>
       <c r="G47" s="24">
-        <v>1.07</v>
+        <v>1.04</v>
       </c>
       <c r="H47" s="25">
         <f t="shared" si="1"/>
-        <v>2.9383777685209667E-2</v>
+        <v>1.703333929878037E-2</v>
       </c>
       <c r="J47" s="9"/>
-      <c r="K47" s="7"/>
+      <c r="K47" s="1"/>
       <c r="L47" s="9"/>
       <c r="M47" s="10"/>
       <c r="N47" s="10"/>
@@ -2335,7 +2332,7 @@
       <c r="P47" s="10"/>
       <c r="Q47" s="13"/>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:17">
       <c r="B48" s="15" t="s">
         <v>98</v>
       </c>
@@ -2349,14 +2346,14 @@
         <v>9</v>
       </c>
       <c r="F48" s="21">
-        <v>0.314419</v>
+        <v>0.26327699999999998</v>
       </c>
       <c r="G48" s="24">
-        <v>1.04</v>
+        <v>1.07</v>
       </c>
       <c r="H48" s="25">
         <f t="shared" si="1"/>
-        <v>1.703333929878037E-2</v>
+        <v>2.9383777685209667E-2</v>
       </c>
       <c r="J48" s="9"/>
       <c r="K48" s="1"/>
@@ -2367,7 +2364,7 @@
       <c r="P48" s="10"/>
       <c r="Q48" s="13"/>
     </row>
-    <row r="49" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:17">
       <c r="B49" s="15" t="s">
         <v>100</v>
       </c>
@@ -2375,20 +2372,20 @@
         <v>101</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F49" s="21">
-        <v>0.26327699999999998</v>
+        <v>0.42303299999999999</v>
       </c>
       <c r="G49" s="24">
-        <v>1.07</v>
+        <v>1.06</v>
       </c>
       <c r="H49" s="25">
         <f t="shared" si="1"/>
-        <v>2.9383777685209667E-2</v>
+        <v>2.5305865264770262E-2</v>
       </c>
       <c r="J49" s="9"/>
       <c r="K49" s="1"/>
@@ -2399,7 +2396,7 @@
       <c r="P49" s="10"/>
       <c r="Q49" s="13"/>
     </row>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:17">
       <c r="B50" s="15" t="s">
         <v>102</v>
       </c>
@@ -2407,20 +2404,20 @@
         <v>103</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E50" s="24" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F50" s="21">
-        <v>0.42303299999999999</v>
+        <v>0.58583099999999999</v>
       </c>
       <c r="G50" s="24">
-        <v>1.06</v>
+        <v>1.08</v>
       </c>
       <c r="H50" s="25">
         <f t="shared" si="1"/>
-        <v>2.5305865264770262E-2</v>
+        <v>3.342375548694973E-2</v>
       </c>
       <c r="J50" s="9"/>
       <c r="K50" s="1"/>
@@ -2431,31 +2428,31 @@
       <c r="P50" s="10"/>
       <c r="Q50" s="13"/>
     </row>
-    <row r="51" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B51" s="15" t="s">
+    <row r="51" spans="2:17">
+      <c r="B51" s="23" t="s">
         <v>104</v>
       </c>
       <c r="C51" s="15" t="s">
         <v>105</v>
       </c>
       <c r="D51" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E51" s="24" t="s">
-        <v>8</v>
-      </c>
       <c r="F51" s="21">
-        <v>0.58583099999999999</v>
+        <v>0.44026399999999999</v>
       </c>
       <c r="G51" s="24">
-        <v>1.08</v>
+        <v>1.05</v>
       </c>
       <c r="H51" s="25">
         <f t="shared" si="1"/>
-        <v>3.342375548694973E-2</v>
+        <v>2.1189299069938092E-2</v>
       </c>
       <c r="J51" s="9"/>
-      <c r="K51" s="1"/>
+      <c r="K51" s="7"/>
       <c r="L51" s="9"/>
       <c r="M51" s="10"/>
       <c r="N51" s="10"/>
@@ -2463,21 +2460,21 @@
       <c r="P51" s="10"/>
       <c r="Q51" s="13"/>
     </row>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B52" s="23" t="s">
+    <row r="52" spans="2:17">
+      <c r="B52" s="15" t="s">
         <v>106</v>
       </c>
       <c r="C52" s="15" t="s">
         <v>107</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E52" s="24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F52" s="21">
-        <v>0.44026399999999999</v>
+        <v>0.349997</v>
       </c>
       <c r="G52" s="24">
         <v>1.05</v>
@@ -2487,7 +2484,7 @@
         <v>2.1189299069938092E-2</v>
       </c>
       <c r="J52" s="9"/>
-      <c r="K52" s="7"/>
+      <c r="K52" s="1"/>
       <c r="L52" s="9"/>
       <c r="M52" s="10"/>
       <c r="N52" s="10"/>
@@ -2495,7 +2492,7 @@
       <c r="P52" s="10"/>
       <c r="Q52" s="13"/>
     </row>
-    <row r="53" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:17">
       <c r="B53" s="15" t="s">
         <v>108</v>
       </c>
@@ -2503,20 +2500,20 @@
         <v>109</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E53" s="24" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F53" s="21">
-        <v>0.349997</v>
+        <v>0.61133000000000004</v>
       </c>
       <c r="G53" s="24">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="H53" s="25">
         <f t="shared" si="1"/>
-        <v>2.1189299069938092E-2</v>
+        <v>1.2837224705172217E-2</v>
       </c>
       <c r="J53" s="9"/>
       <c r="K53" s="1"/>
@@ -2527,7 +2524,7 @@
       <c r="P53" s="10"/>
       <c r="Q53" s="13"/>
     </row>
-    <row r="54" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:17">
       <c r="B54" s="15" t="s">
         <v>110</v>
       </c>
@@ -2535,20 +2532,20 @@
         <v>111</v>
       </c>
       <c r="D54" s="24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E54" s="24" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F54" s="21">
-        <v>0.61133000000000004</v>
+        <v>0.51327199999999995</v>
       </c>
       <c r="G54" s="24">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="H54" s="25">
         <f t="shared" si="1"/>
-        <v>1.2837224705172217E-2</v>
+        <v>1.703333929878037E-2</v>
       </c>
       <c r="J54" s="9"/>
       <c r="K54" s="1"/>
@@ -2559,7 +2556,7 @@
       <c r="P54" s="10"/>
       <c r="Q54" s="13"/>
     </row>
-    <row r="55" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:17">
       <c r="B55" s="15" t="s">
         <v>112</v>
       </c>
@@ -2567,20 +2564,20 @@
         <v>113</v>
       </c>
       <c r="D55" s="24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E55" s="24" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F55" s="21">
-        <v>0.51327199999999995</v>
+        <v>0.89962200000000003</v>
       </c>
       <c r="G55" s="24">
-        <v>1.04</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="H55" s="25">
         <f t="shared" si="1"/>
-        <v>1.703333929878037E-2</v>
+        <v>5.6904851336472557E-2</v>
       </c>
       <c r="J55" s="9"/>
       <c r="K55" s="1"/>
@@ -2591,7 +2588,7 @@
       <c r="P55" s="10"/>
       <c r="Q55" s="13"/>
     </row>
-    <row r="56" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:17">
       <c r="B56" s="15" t="s">
         <v>114</v>
       </c>
@@ -2605,14 +2602,14 @@
         <v>15</v>
       </c>
       <c r="F56" s="21">
-        <v>0.89962200000000003</v>
+        <v>0.16603599999999999</v>
       </c>
       <c r="G56" s="24">
-        <v>1.1399999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H56" s="25">
         <f t="shared" si="1"/>
-        <v>5.6904851336472557E-2</v>
+        <v>4.1392685158225077E-2</v>
       </c>
       <c r="J56" s="9"/>
       <c r="K56" s="1"/>
@@ -2623,7 +2620,7 @@
       <c r="P56" s="10"/>
       <c r="Q56" s="13"/>
     </row>
-    <row r="57" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:17">
       <c r="B57" s="15" t="s">
         <v>116</v>
       </c>
@@ -2631,20 +2628,20 @@
         <v>117</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E57" s="24" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F57" s="21">
-        <v>0.16603599999999999</v>
+        <v>0.121186</v>
       </c>
       <c r="G57" s="24">
-        <v>1.1000000000000001</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="H57" s="25">
         <f t="shared" si="1"/>
-        <v>4.1392685158225077E-2</v>
+        <v>5.6904851336472557E-2</v>
       </c>
       <c r="J57" s="9"/>
       <c r="K57" s="1"/>
@@ -2655,50 +2652,43 @@
       <c r="P57" s="10"/>
       <c r="Q57" s="13"/>
     </row>
-    <row r="58" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:17">
       <c r="B58" s="15" t="s">
         <v>118</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="D58" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="E58" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" s="21">
-        <v>0.121186</v>
-      </c>
-      <c r="G58" s="24">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="H58" s="25">
-        <f t="shared" si="1"/>
-        <v>5.6904851336472557E-2</v>
-      </c>
+      <c r="D58" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" s="26"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="26"/>
       <c r="J58" s="9"/>
-      <c r="K58" s="1"/>
+      <c r="K58" s="9"/>
       <c r="L58" s="9"/>
-      <c r="M58" s="10"/>
-      <c r="N58" s="10"/>
-      <c r="O58" s="8"/>
-      <c r="P58" s="10"/>
-      <c r="Q58" s="13"/>
-    </row>
-    <row r="59" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="M58" s="14"/>
+      <c r="N58" s="14"/>
+      <c r="O58" s="14"/>
+      <c r="P58" s="14"/>
+      <c r="Q58" s="14"/>
+    </row>
+    <row r="59" spans="2:17">
       <c r="B59" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D59" s="26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E59" s="26" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F59" s="26"/>
       <c r="G59" s="26"/>
@@ -2712,40 +2702,15 @@
       <c r="P59" s="14"/>
       <c r="Q59" s="14"/>
     </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B60" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C60" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="D60" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E60" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F60" s="26"/>
-      <c r="G60" s="26"/>
-      <c r="H60" s="26"/>
+    <row r="60" spans="2:17">
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
       <c r="L60" s="9"/>
-      <c r="M60" s="14"/>
-      <c r="N60" s="14"/>
-      <c r="O60" s="14"/>
-      <c r="P60" s="14"/>
-      <c r="Q60" s="14"/>
-    </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="J61" s="9"/>
-      <c r="K61" s="9"/>
-      <c r="L61" s="9"/>
-      <c r="M61" s="9"/>
-      <c r="N61" s="9"/>
-      <c r="O61" s="9"/>
-      <c r="P61" s="9"/>
-      <c r="Q61" s="9"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="9"/>
+      <c r="O60" s="9"/>
+      <c r="P60" s="9"/>
+      <c r="Q60" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated - now added ncode to incorporate newgwas
</commit_message>
<xml_diff>
--- a/inputs/SNP_info.xlsx
+++ b/inputs/SNP_info.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/tb13101/Desktop/Mini-project 1/Files_for_paper/CAD_adolescent_analysis/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D21C7A4-0F2C-6444-ACF0-2034E45CE83A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1180" windowWidth="28160" windowHeight="15320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="2740" windowWidth="28160" windowHeight="15320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -836,7 +837,7 @@
   <dimension ref="B1:Q60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>